<commit_message>
boeketten toevoegen en boekingen controller
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Documents\GitHub\Flowerpower\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{ED3291D0-4A2A-4BD1-BE70-D5B53FBF74B4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{96B86C76-5F5B-41FC-A01F-A8E17B78F71C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{2EB69A4A-0AF8-495A-BCB0-F8D4EFA32CF2}"/>
   </bookViews>
@@ -620,7 +620,7 @@
   <dimension ref="F6:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20:N20"/>
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,14 +652,16 @@
     </row>
     <row r="7" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F7" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="5" t="s">
-        <v>29</v>
+      <c r="H7" s="4">
+        <v>43385</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="J7" s="1">
         <v>1</v>
@@ -672,7 +674,7 @@
       <c r="G8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="H8" s="4"/>
       <c r="I8" s="5" t="s">
         <v>29</v>
       </c>
@@ -687,7 +689,7 @@
       <c r="G9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="4"/>
       <c r="I9" s="5" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
mooiste update van je welkomst
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Flowerpower\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72498121-2290-4A0E-BC6B-A3BDA9E8161C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1B7C6D-6628-4456-9CC0-A7EF6A02E83E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{2EB69A4A-0AF8-495A-BCB0-F8D4EFA32CF2}"/>
   </bookViews>
@@ -629,7 +629,7 @@
   <dimension ref="F6:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,9 +717,11 @@
       <c r="G10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="5" t="s">
-        <v>29</v>
+      <c r="H10" s="4">
+        <v>43391</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="J10" s="1">
         <v>1</v>
@@ -777,9 +779,11 @@
       <c r="G14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="5" t="s">
-        <v>29</v>
+      <c r="H14" s="4">
+        <v>43391</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="J14" s="1">
         <v>2</v>
@@ -856,9 +860,11 @@
       <c r="G19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="5" t="s">
-        <v>29</v>
+      <c r="H19" s="4">
+        <v>43391</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="J19" s="1">
         <v>3</v>
@@ -888,9 +894,11 @@
       <c r="G21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="5" t="s">
-        <v>29</v>
+      <c r="H21" s="4">
+        <v>43391</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="J21" s="1">
         <v>3</v>
@@ -903,9 +911,11 @@
       <c r="G22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="5" t="s">
-        <v>29</v>
+      <c r="H22" s="4">
+        <v>43391</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="J22" s="1">
         <v>3</v>

</xml_diff>